<commit_message>
changed color scheme - black mask, white legend
</commit_message>
<xml_diff>
--- a/kicad/kicad_8x8_45/PCB Technology Requirement Format V1 for ultim8x8.xlsx
+++ b/kicad/kicad_8x8_45/PCB Technology Requirement Format V1 for ultim8x8.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -26,12 +26,76 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">                         深圳矽递科技有限公司
+                          </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>                         深圳矽递科技有限公司
-                          </t>
+      <t xml:space="preserve">Seeed Technology Limited</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB Technology Requirement Format</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB Name &amp; Version</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ULTiM8x8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PCB Material
+PCB</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">板材：</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">  
+    (Rigid)FR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">－</t>
     </r>
     <r>
       <rPr>
@@ -41,29 +105,21 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>Seeed Technology Limited</t>
-    </r>
-  </si>
-  <si>
-    <t>PCB Technology Requirement Format</t>
-  </si>
-  <si>
-    <t>PCB Name &amp; Version</t>
-  </si>
-  <si>
-    <t>ULTiM8x8</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>PCB Material
+      <t xml:space="preserve">4
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PCB Size
 PCB</t>
     </r>
     <r>
@@ -71,142 +127,107 @@
         <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>板材：</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>  
-    (Rigid)FR</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>－</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>4
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">大小：</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> inch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( 2.40 ) × (2.40 )</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PCB  Layer
+PCB</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">层数：</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Thickness
+PCB</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">厚度：</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1.6mm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Copper Weight
 </t>
     </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>PCB Size
-PCB</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>大小：</t>
-    </r>
-  </si>
-  <si>
-    <t> inch</t>
-  </si>
-  <si>
-    <t>( 2.40 ) × (2.40 )</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>PCB  Layer
-PCB</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>层数：</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Thickness
-PCB</t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>厚度：</t>
-    </r>
-  </si>
-  <si>
-    <t>1.6mm</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Copper Weight
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">铜厚：</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1oz</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">PCB Colour
 </t>
     </r>
     <r>
@@ -214,27 +235,23 @@
         <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>铜厚：</t>
-    </r>
-  </si>
-  <si>
-    <t>1oz</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>PCB Colour
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">阻焊颜色：</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Black
 </t>
     </r>
     <r>
@@ -242,46 +259,23 @@
         <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>阻焊颜色：</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>White</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>白色</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Silkscreen
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">黑色</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Silkscreen
 </t>
     </r>
     <r>
@@ -289,50 +283,50 @@
         <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>字符颜色：</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Black
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">字符颜色：</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">White
 </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>黑色</t>
-    </r>
-  </si>
-  <si>
-    <t>other:(            )</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Pads Finished
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">白色</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">other:(            )</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Pads Finished
 </t>
     </r>
     <r>
@@ -340,47 +334,45 @@
         <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>焊盘喷镀：</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> (Hasl-lead free)   
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">焊盘喷镀：</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> (Hasl-lead free)   
 </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>无铅喷锡</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Via solder mask
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">无铅喷锡</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Via solder mask
 </t>
     </r>
     <r>
@@ -388,47 +380,45 @@
         <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>阻焊覆盖：</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>solder mask  opening 
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">阻焊覆盖：</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">solder mask  opening 
 </t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>过孔开窗</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Minimum trace/space
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">过孔开窗</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Minimum trace/space
 (mm)
 </t>
     </r>
@@ -437,27 +427,26 @@
         <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>最小线宽</t>
-    </r>
-  </si>
-  <si>
-    <t>0.254mm/0.254mm</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Minimum hole size
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">最小线宽</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">0.254mm/0.254mm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Minimum hole size
 (mm)
 </t>
     </r>
@@ -466,27 +455,26 @@
         <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>最小孔径</t>
-    </r>
-  </si>
-  <si>
-    <t>0.635mm</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>Special requirements
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">最小孔径</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">0.635mm</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Special requirements
 </t>
     </r>
     <r>
@@ -494,21 +482,20 @@
         <b val="true"/>
         <sz val="11"/>
         <color rgb="FF000000"/>
-        <rFont val="Droid Sans Fallback"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>特殊工艺：</t>
-    </r>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>(Put requirements here)</t>
-  </si>
-  <si>
-    <t>Comment:</t>
+        <rFont val="Noto Sans CJK SC Regular"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">特殊工艺：</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Put requirements here)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Comment:</t>
   </si>
 </sst>
 </file>
@@ -516,10 +503,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0_ "/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -545,9 +532,8 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Droid Sans Fallback"/>
+      <name val="Noto Sans CJK SC Regular"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -582,6 +568,20 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC Regular"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Droid Sans Fallback"/>
@@ -734,7 +734,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -759,11 +759,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -775,11 +775,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -803,28 +803,36 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -922,9 +930,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>724320</xdr:colOff>
+      <xdr:colOff>723960</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>466920</xdr:rowOff>
+      <xdr:rowOff>466560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -938,7 +946,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="92160" y="29520"/>
-          <a:ext cx="632160" cy="437400"/>
+          <a:ext cx="631800" cy="437040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -961,18 +969,18 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.2226720647773"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="20.9109311740891"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="19.6234817813765"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.5951417004049"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.9676113360324"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.080971659919"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.68421052631579"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.0242914979757"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="22.4534412955466"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.080971659919"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9676113360324"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="24.6801619433198"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.1983805668016"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="10.3684210526316"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1099,10 +1107,10 @@
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>15</v>
       </c>
+      <c r="C10" s="18"/>
       <c r="D10" s="19"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
@@ -1111,22 +1119,22 @@
     </row>
     <row r="11" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
-      <c r="B11" s="17"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="18"/>
       <c r="D11" s="12"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
       <c r="H11" s="16"/>
     </row>
     <row r="12" customFormat="false" ht="34.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="18" t="s">
+      <c r="B12" s="17" t="s">
         <v>17</v>
       </c>
+      <c r="C12" s="18"/>
       <c r="D12" s="12" t="s">
         <v>18</v>
       </c>
@@ -1135,7 +1143,7 @@
       <c r="A13" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="22" t="s">
         <v>20</v>
       </c>
       <c r="C13" s="18"/>
@@ -1145,20 +1153,20 @@
       <c r="A14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18" t="s">
+      <c r="B14" s="20"/>
+      <c r="C14" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="21"/>
+      <c r="D14" s="24"/>
     </row>
     <row r="15" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="12" t="s">
@@ -1172,18 +1180,18 @@
       <c r="B16" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="24"/>
     </row>
     <row r="17" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="s">
+      <c r="A17" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>